<commit_message>
Added Notes column to explain some changes
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-red-hat-enterprise-linux-7-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-red-hat-enterprise-linux-7-stig-overlay.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\CMS_InSpec_Profile_to_NISTSecurityControl_Maps_06132019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110F197C-A3BB-42BC-9C9A-0145E9B84F27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72436B3B-B88E-4534-B2C2-904A19ACB433}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'rhel7-output'!$A$1:$AB$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'rhel7-output'!$A$1:$AC$243</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$C$239</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4113" uniqueCount="1861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="1863">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -9175,12 +9175,18 @@
   <si>
     <t>NIST</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMS ARS 3.1 does not use IA-11, however traditionally this type of finding is associated with AC-6, Least Privilege. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9327,6 +9333,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9700,7 +9713,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -9755,6 +9768,21 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -10111,13 +10139,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU243"/>
+  <dimension ref="A1:AC243"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10148,13 +10176,14 @@
     <col min="24" max="24" width="24.1015625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11.20703125" style="1" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="11.20703125" style="18" customWidth="1"/>
-    <col min="27" max="27" width="13.1015625" style="1" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="14.20703125" style="1" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="8.89453125" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.89453125" style="1"/>
+    <col min="27" max="27" width="21" style="18" customWidth="1"/>
+    <col min="28" max="28" width="13.1015625" style="1" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="14.20703125" style="1" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="8.89453125" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -10233,14 +10262,17 @@
       <c r="Z1" s="14" t="s">
         <v>1860</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="19" t="s">
+        <v>1861</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="288" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:29" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -10299,12 +10331,13 @@
       <c r="Z2" s="14" t="s">
         <v>1776</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB2" s="2"/>
-    </row>
-    <row r="3" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -10361,12 +10394,13 @@
       <c r="Z3" s="15" t="s">
         <v>1775</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB3" s="2"/>
-    </row>
-    <row r="4" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC3" s="2"/>
+    </row>
+    <row r="4" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
         <v>52</v>
       </c>
@@ -10425,12 +10459,13 @@
       <c r="Z4" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB4" s="2"/>
-    </row>
-    <row r="5" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC4" s="2"/>
+    </row>
+    <row r="5" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7" t="s">
         <v>58</v>
       </c>
@@ -10489,12 +10524,13 @@
       <c r="Z5" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB5" s="2"/>
-    </row>
-    <row r="6" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC5" s="2"/>
+    </row>
+    <row r="6" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>61</v>
       </c>
@@ -10553,12 +10589,13 @@
       <c r="Z6" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB6" s="2"/>
-    </row>
-    <row r="7" spans="1:28" ht="388.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC6" s="2"/>
+    </row>
+    <row r="7" spans="1:29" ht="388.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>64</v>
       </c>
@@ -10617,12 +10654,13 @@
       <c r="Z7" s="14" t="s">
         <v>1778</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB7" s="2"/>
-    </row>
-    <row r="8" spans="1:28" ht="388.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC7" s="2"/>
+    </row>
+    <row r="8" spans="1:29" ht="388.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>73</v>
       </c>
@@ -10681,12 +10719,13 @@
       <c r="Z8" s="14" t="s">
         <v>1778</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB8" s="2"/>
-    </row>
-    <row r="9" spans="1:28" ht="403.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC8" s="2"/>
+    </row>
+    <row r="9" spans="1:29" ht="403.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="11" t="s">
         <v>82</v>
       </c>
@@ -10745,12 +10784,13 @@
       <c r="Z9" s="14" t="s">
         <v>1778</v>
       </c>
-      <c r="AA9" s="2" t="s">
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB9" s="2"/>
-    </row>
-    <row r="10" spans="1:28" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC9" s="2"/>
+    </row>
+    <row r="10" spans="1:29" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
         <v>88</v>
       </c>
@@ -10809,12 +10849,13 @@
       <c r="Z10" s="14" t="s">
         <v>1778</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB10" s="2"/>
-    </row>
-    <row r="11" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC10" s="2"/>
+    </row>
+    <row r="11" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>95</v>
       </c>
@@ -10873,12 +10914,13 @@
       <c r="Z11" s="14" t="s">
         <v>1778</v>
       </c>
-      <c r="AA11" s="2" t="s">
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB11" s="2"/>
-    </row>
-    <row r="12" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC11" s="2"/>
+    </row>
+    <row r="12" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7" t="s">
         <v>101</v>
       </c>
@@ -10937,12 +10979,13 @@
       <c r="Z12" s="14" t="s">
         <v>1778</v>
       </c>
-      <c r="AA12" s="2" t="s">
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB12" s="2"/>
-    </row>
-    <row r="13" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC12" s="2"/>
+    </row>
+    <row r="13" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
         <v>107</v>
       </c>
@@ -11001,12 +11044,13 @@
       <c r="Z13" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA13" s="2" t="s">
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB13" s="2"/>
-    </row>
-    <row r="14" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC13" s="2"/>
+    </row>
+    <row r="14" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7" t="s">
         <v>116</v>
       </c>
@@ -11065,12 +11109,13 @@
       <c r="Z14" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA14" s="2" t="s">
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB14" s="2"/>
-    </row>
-    <row r="15" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC14" s="2"/>
+    </row>
+    <row r="15" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
         <v>124</v>
       </c>
@@ -11129,12 +11174,13 @@
       <c r="Z15" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA15" s="2" t="s">
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB15" s="2"/>
-    </row>
-    <row r="16" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC15" s="2"/>
+    </row>
+    <row r="16" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7" t="s">
         <v>132</v>
       </c>
@@ -11193,12 +11239,13 @@
       <c r="Z16" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA16" s="2" t="s">
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB16" s="2"/>
-    </row>
-    <row r="17" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC16" s="2"/>
+    </row>
+    <row r="17" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7" t="s">
         <v>140</v>
       </c>
@@ -11257,12 +11304,13 @@
       <c r="Z17" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA17" s="2" t="s">
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB17" s="2"/>
-    </row>
-    <row r="18" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC17" s="2"/>
+    </row>
+    <row r="18" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="7" t="s">
         <v>148</v>
       </c>
@@ -11321,12 +11369,13 @@
       <c r="Z18" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA18" s="2" t="s">
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB18" s="2"/>
-    </row>
-    <row r="19" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC18" s="2"/>
+    </row>
+    <row r="19" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="7" t="s">
         <v>154</v>
       </c>
@@ -11385,12 +11434,13 @@
       <c r="Z19" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA19" s="2" t="s">
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB19" s="2"/>
-    </row>
-    <row r="20" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC19" s="2"/>
+    </row>
+    <row r="20" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7" t="s">
         <v>160</v>
       </c>
@@ -11449,12 +11499,13 @@
       <c r="Z20" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA20" s="2" t="s">
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB20" s="2"/>
-    </row>
-    <row r="21" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC20" s="2"/>
+    </row>
+    <row r="21" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5" t="s">
         <v>166</v>
       </c>
@@ -11513,12 +11564,13 @@
       <c r="Z21" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA21" s="2" t="s">
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB21" s="2"/>
-    </row>
-    <row r="22" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC21" s="2"/>
+    </row>
+    <row r="22" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5" t="s">
         <v>175</v>
       </c>
@@ -11577,12 +11629,13 @@
       <c r="Z22" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA22" s="2" t="s">
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB22" s="2"/>
-    </row>
-    <row r="23" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC22" s="2"/>
+    </row>
+    <row r="23" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5" t="s">
         <v>181</v>
       </c>
@@ -11641,12 +11694,13 @@
       <c r="Z23" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA23" s="2" t="s">
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB23" s="2"/>
-    </row>
-    <row r="24" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC23" s="2"/>
+    </row>
+    <row r="24" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5" t="s">
         <v>187</v>
       </c>
@@ -11705,12 +11759,13 @@
       <c r="Z24" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA24" s="2" t="s">
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB24" s="2"/>
-    </row>
-    <row r="25" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC24" s="2"/>
+    </row>
+    <row r="25" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5" t="s">
         <v>196</v>
       </c>
@@ -11769,12 +11824,13 @@
       <c r="Z25" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA25" s="2" t="s">
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB25" s="2"/>
-    </row>
-    <row r="26" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC25" s="2"/>
+    </row>
+    <row r="26" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5" t="s">
         <v>202</v>
       </c>
@@ -11833,12 +11889,13 @@
       <c r="Z26" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA26" s="2" t="s">
+      <c r="AA26" s="19"/>
+      <c r="AB26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB26" s="2"/>
-    </row>
-    <row r="27" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC26" s="2"/>
+    </row>
+    <row r="27" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5" t="s">
         <v>211</v>
       </c>
@@ -11897,12 +11954,13 @@
       <c r="Z27" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA27" s="2" t="s">
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB27" s="2"/>
-    </row>
-    <row r="28" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC27" s="2"/>
+    </row>
+    <row r="28" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="7" t="s">
         <v>217</v>
       </c>
@@ -11961,12 +12019,13 @@
       <c r="Z28" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA28" s="2" t="s">
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB28" s="2"/>
-    </row>
-    <row r="29" spans="1:28" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC28" s="2"/>
+    </row>
+    <row r="29" spans="1:29" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="7" t="s">
         <v>226</v>
       </c>
@@ -12025,12 +12084,13 @@
       <c r="Z29" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA29" s="2" t="s">
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB29" s="2"/>
-    </row>
-    <row r="30" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC29" s="2"/>
+    </row>
+    <row r="30" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5" t="s">
         <v>235</v>
       </c>
@@ -12089,12 +12149,13 @@
       <c r="Z30" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA30" s="2" t="s">
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB30" s="2"/>
-    </row>
-    <row r="31" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC30" s="2"/>
+    </row>
+    <row r="31" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="7" t="s">
         <v>243</v>
       </c>
@@ -12153,12 +12214,13 @@
       <c r="Z31" s="14" t="s">
         <v>1783</v>
       </c>
-      <c r="AA31" s="2" t="s">
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB31" s="2"/>
-    </row>
-    <row r="32" spans="1:28" ht="313.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC31" s="2"/>
+    </row>
+    <row r="32" spans="1:29" ht="313.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="7" t="s">
         <v>252</v>
       </c>
@@ -12217,12 +12279,13 @@
       <c r="Z32" s="14" t="s">
         <v>1782</v>
       </c>
-      <c r="AA32" s="2" t="s">
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB32" s="2"/>
-    </row>
-    <row r="33" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC32" s="2"/>
+    </row>
+    <row r="33" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7" t="s">
         <v>261</v>
       </c>
@@ -12281,12 +12344,13 @@
       <c r="Z33" s="14" t="s">
         <v>1784</v>
       </c>
-      <c r="AA33" s="2" t="s">
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB33" s="2"/>
-    </row>
-    <row r="34" spans="1:28" ht="403.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC33" s="2"/>
+    </row>
+    <row r="34" spans="1:29" ht="403.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="7" t="s">
         <v>272</v>
       </c>
@@ -12345,12 +12409,13 @@
       <c r="Z34" s="14" t="s">
         <v>1784</v>
       </c>
-      <c r="AA34" s="2" t="s">
+      <c r="AA34" s="19"/>
+      <c r="AB34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB34" s="2"/>
-    </row>
-    <row r="35" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC34" s="2"/>
+    </row>
+    <row r="35" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="7" t="s">
         <v>280</v>
       </c>
@@ -12409,12 +12474,15 @@
       <c r="Z35" s="15" t="s">
         <v>1820</v>
       </c>
-      <c r="AA35" s="2" t="s">
+      <c r="AA35" s="23" t="s">
+        <v>1862</v>
+      </c>
+      <c r="AB35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB35" s="2"/>
-    </row>
-    <row r="36" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC35" s="2"/>
+    </row>
+    <row r="36" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7" t="s">
         <v>289</v>
       </c>
@@ -12473,12 +12541,15 @@
       <c r="Z36" s="15" t="s">
         <v>1820</v>
       </c>
-      <c r="AA36" s="2" t="s">
+      <c r="AA36" s="23" t="s">
+        <v>1862</v>
+      </c>
+      <c r="AB36" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB36" s="2"/>
-    </row>
-    <row r="37" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC36" s="2"/>
+    </row>
+    <row r="37" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="7" t="s">
         <v>296</v>
       </c>
@@ -12537,12 +12608,13 @@
       <c r="Z37" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA37" s="2" t="s">
+      <c r="AA37" s="19"/>
+      <c r="AB37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB37" s="2"/>
-    </row>
-    <row r="38" spans="1:28" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC37" s="2"/>
+    </row>
+    <row r="38" spans="1:29" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="5" t="s">
         <v>303</v>
       </c>
@@ -12601,12 +12673,13 @@
       <c r="Z38" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA38" s="2" t="s">
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB38" s="2"/>
-    </row>
-    <row r="39" spans="1:28" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC38" s="2"/>
+    </row>
+    <row r="39" spans="1:29" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="5" t="s">
         <v>311</v>
       </c>
@@ -12665,12 +12738,13 @@
       <c r="Z39" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA39" s="2" t="s">
+      <c r="AA39" s="19"/>
+      <c r="AB39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB39" s="2"/>
-    </row>
-    <row r="40" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC39" s="2"/>
+    </row>
+    <row r="40" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="5" t="s">
         <v>317</v>
       </c>
@@ -12729,12 +12803,13 @@
       <c r="Z40" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA40" s="2" t="s">
+      <c r="AA40" s="19"/>
+      <c r="AB40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB40" s="2"/>
-    </row>
-    <row r="41" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC40" s="2"/>
+    </row>
+    <row r="41" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="5" t="s">
         <v>323</v>
       </c>
@@ -12793,12 +12868,13 @@
       <c r="Z41" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA41" s="2" t="s">
+      <c r="AA41" s="19"/>
+      <c r="AB41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB41" s="2"/>
-    </row>
-    <row r="42" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC41" s="2"/>
+    </row>
+    <row r="42" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="5" t="s">
         <v>329</v>
       </c>
@@ -12857,12 +12933,13 @@
       <c r="Z42" s="14" t="s">
         <v>1785</v>
       </c>
-      <c r="AA42" s="2" t="s">
+      <c r="AA42" s="19"/>
+      <c r="AB42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB42" s="2"/>
-    </row>
-    <row r="43" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC42" s="2"/>
+    </row>
+    <row r="43" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="5" t="s">
         <v>338</v>
       </c>
@@ -12921,12 +12998,13 @@
       <c r="Z43" s="14" t="s">
         <v>1785</v>
       </c>
-      <c r="AA43" s="2" t="s">
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB43" s="2"/>
-    </row>
-    <row r="44" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC43" s="2"/>
+    </row>
+    <row r="44" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="5" t="s">
         <v>344</v>
       </c>
@@ -12985,12 +13063,13 @@
       <c r="Z44" s="14" t="s">
         <v>1783</v>
       </c>
-      <c r="AA44" s="2" t="s">
+      <c r="AA44" s="19"/>
+      <c r="AB44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB44" s="2"/>
-    </row>
-    <row r="45" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC44" s="2"/>
+    </row>
+    <row r="45" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="5" t="s">
         <v>352</v>
       </c>
@@ -13049,12 +13128,13 @@
       <c r="Z45" s="14" t="s">
         <v>1786</v>
       </c>
-      <c r="AA45" s="2" t="s">
+      <c r="AA45" s="19"/>
+      <c r="AB45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB45" s="2"/>
-    </row>
-    <row r="46" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC45" s="2"/>
+    </row>
+    <row r="46" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5" t="s">
         <v>361</v>
       </c>
@@ -13113,12 +13193,13 @@
       <c r="Z46" s="14" t="s">
         <v>1786</v>
       </c>
-      <c r="AA46" s="2" t="s">
+      <c r="AA46" s="19"/>
+      <c r="AB46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB46" s="2"/>
-    </row>
-    <row r="47" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC46" s="2"/>
+    </row>
+    <row r="47" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7" t="s">
         <v>368</v>
       </c>
@@ -13177,12 +13258,13 @@
       <c r="Z47" s="14" t="s">
         <v>1820</v>
       </c>
-      <c r="AA47" s="2" t="s">
+      <c r="AA47" s="19"/>
+      <c r="AB47" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB47" s="2"/>
-    </row>
-    <row r="48" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC47" s="2"/>
+    </row>
+    <row r="48" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="7" t="s">
         <v>377</v>
       </c>
@@ -13241,12 +13323,13 @@
       <c r="Z48" s="15" t="s">
         <v>1793</v>
       </c>
-      <c r="AA48" s="2" t="s">
+      <c r="AA48" s="20"/>
+      <c r="AB48" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB48" s="2"/>
-    </row>
-    <row r="49" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC48" s="2"/>
+    </row>
+    <row r="49" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="7" t="s">
         <v>386</v>
       </c>
@@ -13305,12 +13388,13 @@
       <c r="Z49" s="15" t="s">
         <v>1796</v>
       </c>
-      <c r="AA49" s="2" t="s">
+      <c r="AA49" s="20"/>
+      <c r="AB49" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB49" s="2"/>
-    </row>
-    <row r="50" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC49" s="2"/>
+    </row>
+    <row r="50" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="7" t="s">
         <v>392</v>
       </c>
@@ -13369,12 +13453,13 @@
       <c r="Z50" s="15" t="s">
         <v>1797</v>
       </c>
-      <c r="AA50" s="2" t="s">
+      <c r="AA50" s="20"/>
+      <c r="AB50" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB50" s="2"/>
-    </row>
-    <row r="51" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC50" s="2"/>
+    </row>
+    <row r="51" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="7" t="s">
         <v>401</v>
       </c>
@@ -13433,12 +13518,13 @@
       <c r="Z51" s="15" t="s">
         <v>1797</v>
       </c>
-      <c r="AA51" s="2" t="s">
+      <c r="AA51" s="20"/>
+      <c r="AB51" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB51" s="2"/>
-    </row>
-    <row r="52" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC51" s="2"/>
+    </row>
+    <row r="52" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="7" t="s">
         <v>407</v>
       </c>
@@ -13497,12 +13583,13 @@
       <c r="Z52" s="15" t="s">
         <v>1797</v>
       </c>
-      <c r="AA52" s="2" t="s">
+      <c r="AA52" s="20"/>
+      <c r="AB52" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB52" s="2"/>
-    </row>
-    <row r="53" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC52" s="2"/>
+    </row>
+    <row r="53" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="5" t="s">
         <v>414</v>
       </c>
@@ -13561,12 +13648,13 @@
       <c r="Z53" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA53" s="2" t="s">
+      <c r="AA53" s="19"/>
+      <c r="AB53" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB53" s="2"/>
-    </row>
-    <row r="54" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC53" s="2"/>
+    </row>
+    <row r="54" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="5" t="s">
         <v>423</v>
       </c>
@@ -13625,12 +13713,13 @@
       <c r="Z54" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA54" s="2" t="s">
+      <c r="AA54" s="19"/>
+      <c r="AB54" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB54" s="2"/>
-    </row>
-    <row r="55" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC54" s="2"/>
+    </row>
+    <row r="55" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="7" t="s">
         <v>430</v>
       </c>
@@ -13689,12 +13778,13 @@
       <c r="Z55" s="14" t="s">
         <v>1799</v>
       </c>
-      <c r="AA55" s="2" t="s">
+      <c r="AA55" s="19"/>
+      <c r="AB55" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB55" s="2"/>
-    </row>
-    <row r="56" spans="1:28" ht="403.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC55" s="2"/>
+    </row>
+    <row r="56" spans="1:29" ht="403.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="7" t="s">
         <v>441</v>
       </c>
@@ -13753,12 +13843,13 @@
       <c r="Z56" s="14" t="s">
         <v>1800</v>
       </c>
-      <c r="AA56" s="2" t="s">
+      <c r="AA56" s="19"/>
+      <c r="AB56" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB56" s="2"/>
-    </row>
-    <row r="57" spans="1:28" ht="403.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC56" s="2"/>
+    </row>
+    <row r="57" spans="1:29" ht="403.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="7" t="s">
         <v>450</v>
       </c>
@@ -13817,12 +13908,13 @@
       <c r="Z57" s="14" t="s">
         <v>1800</v>
       </c>
-      <c r="AA57" s="2" t="s">
+      <c r="AA57" s="19"/>
+      <c r="AB57" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB57" s="2"/>
-    </row>
-    <row r="58" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC57" s="2"/>
+    </row>
+    <row r="58" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="5" t="s">
         <v>456</v>
       </c>
@@ -13881,12 +13973,13 @@
       <c r="Z58" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA58" s="2" t="s">
+      <c r="AA58" s="19"/>
+      <c r="AB58" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB58" s="2"/>
-    </row>
-    <row r="59" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC58" s="2"/>
+    </row>
+    <row r="59" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="5" t="s">
         <v>463</v>
       </c>
@@ -13945,12 +14038,13 @@
       <c r="Z59" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA59" s="2" t="s">
+      <c r="AA59" s="19"/>
+      <c r="AB59" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB59" s="2"/>
-    </row>
-    <row r="60" spans="1:28" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC59" s="2"/>
+    </row>
+    <row r="60" spans="1:29" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="5" t="s">
         <v>471</v>
       </c>
@@ -14009,12 +14103,13 @@
       <c r="Z60" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA60" s="2" t="s">
+      <c r="AA60" s="19"/>
+      <c r="AB60" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB60" s="2"/>
-    </row>
-    <row r="61" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC60" s="2"/>
+    </row>
+    <row r="61" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="5" t="s">
         <v>478</v>
       </c>
@@ -14073,12 +14168,13 @@
       <c r="Z61" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA61" s="2" t="s">
+      <c r="AA61" s="19"/>
+      <c r="AB61" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB61" s="2"/>
-    </row>
-    <row r="62" spans="1:28" ht="388.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC61" s="2"/>
+    </row>
+    <row r="62" spans="1:29" ht="388.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="5" t="s">
         <v>485</v>
       </c>
@@ -14137,12 +14233,13 @@
       <c r="Z62" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA62" s="2" t="s">
+      <c r="AA62" s="19"/>
+      <c r="AB62" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB62" s="2"/>
-    </row>
-    <row r="63" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC62" s="2"/>
+    </row>
+    <row r="63" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="5" t="s">
         <v>492</v>
       </c>
@@ -14201,12 +14298,13 @@
       <c r="Z63" s="14" t="s">
         <v>1781</v>
       </c>
-      <c r="AA63" s="2" t="s">
+      <c r="AA63" s="19"/>
+      <c r="AB63" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB63" s="2"/>
-    </row>
-    <row r="64" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC63" s="2"/>
+    </row>
+    <row r="64" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="5" t="s">
         <v>500</v>
       </c>
@@ -14265,12 +14363,13 @@
       <c r="Z64" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA64" s="2" t="s">
+      <c r="AA64" s="19"/>
+      <c r="AB64" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB64" s="2"/>
-    </row>
-    <row r="65" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC64" s="2"/>
+    </row>
+    <row r="65" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="7" t="s">
         <v>507</v>
       </c>
@@ -14329,12 +14428,13 @@
       <c r="Z65" s="15" t="s">
         <v>1785</v>
       </c>
-      <c r="AA65" s="2" t="s">
+      <c r="AA65" s="20"/>
+      <c r="AB65" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB65" s="2"/>
-    </row>
-    <row r="66" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC65" s="2"/>
+    </row>
+    <row r="66" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="7" t="s">
         <v>515</v>
       </c>
@@ -14393,12 +14493,13 @@
       <c r="Z66" s="15" t="s">
         <v>1785</v>
       </c>
-      <c r="AA66" s="2" t="s">
+      <c r="AA66" s="20"/>
+      <c r="AB66" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB66" s="2"/>
-    </row>
-    <row r="67" spans="1:28" ht="331.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC66" s="2"/>
+    </row>
+    <row r="67" spans="1:29" ht="331.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="5" t="s">
         <v>522</v>
       </c>
@@ -14457,12 +14558,13 @@
       <c r="Z67" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA67" s="2" t="s">
+      <c r="AA67" s="19"/>
+      <c r="AB67" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB67" s="2"/>
-    </row>
-    <row r="68" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC67" s="2"/>
+    </row>
+    <row r="68" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="5" t="s">
         <v>529</v>
       </c>
@@ -14521,12 +14623,13 @@
       <c r="Z68" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA68" s="2" t="s">
+      <c r="AA68" s="19"/>
+      <c r="AB68" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB68" s="2"/>
-    </row>
-    <row r="69" spans="1:28" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC68" s="2"/>
+    </row>
+    <row r="69" spans="1:29" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="5" t="s">
         <v>535</v>
       </c>
@@ -14585,12 +14688,13 @@
       <c r="Z69" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA69" s="2" t="s">
+      <c r="AA69" s="19"/>
+      <c r="AB69" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB69" s="2"/>
-    </row>
-    <row r="70" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC69" s="2"/>
+    </row>
+    <row r="70" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="5" t="s">
         <v>542</v>
       </c>
@@ -14649,12 +14753,13 @@
       <c r="Z70" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA70" s="2" t="s">
+      <c r="AA70" s="19"/>
+      <c r="AB70" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB70" s="2"/>
-    </row>
-    <row r="71" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC70" s="2"/>
+    </row>
+    <row r="71" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="5" t="s">
         <v>549</v>
       </c>
@@ -14713,12 +14818,13 @@
       <c r="Z71" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA71" s="2" t="s">
+      <c r="AA71" s="19"/>
+      <c r="AB71" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB71" s="2"/>
-    </row>
-    <row r="72" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC71" s="2"/>
+    </row>
+    <row r="72" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="5" t="s">
         <v>556</v>
       </c>
@@ -14777,12 +14883,13 @@
       <c r="Z72" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA72" s="2" t="s">
+      <c r="AA72" s="19"/>
+      <c r="AB72" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB72" s="2"/>
-    </row>
-    <row r="73" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC72" s="2"/>
+    </row>
+    <row r="73" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="5" t="s">
         <v>563</v>
       </c>
@@ -14841,12 +14948,13 @@
       <c r="Z73" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA73" s="2" t="s">
+      <c r="AA73" s="19"/>
+      <c r="AB73" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB73" s="2"/>
-    </row>
-    <row r="74" spans="1:28" ht="388.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC73" s="2"/>
+    </row>
+    <row r="74" spans="1:29" ht="388.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="5" t="s">
         <v>570</v>
       </c>
@@ -14905,12 +15013,13 @@
       <c r="Z74" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA74" s="2" t="s">
+      <c r="AA74" s="19"/>
+      <c r="AB74" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB74" s="2"/>
-    </row>
-    <row r="75" spans="1:28" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC74" s="2"/>
+    </row>
+    <row r="75" spans="1:29" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="5" t="s">
         <v>577</v>
       </c>
@@ -14969,12 +15078,13 @@
       <c r="Z75" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA75" s="2" t="s">
+      <c r="AA75" s="19"/>
+      <c r="AB75" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB75" s="2"/>
-    </row>
-    <row r="76" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC75" s="2"/>
+    </row>
+    <row r="76" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="5" t="s">
         <v>584</v>
       </c>
@@ -15033,12 +15143,13 @@
       <c r="Z76" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA76" s="2" t="s">
+      <c r="AA76" s="19"/>
+      <c r="AB76" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB76" s="2"/>
-    </row>
-    <row r="77" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC76" s="2"/>
+    </row>
+    <row r="77" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="5" t="s">
         <v>591</v>
       </c>
@@ -15097,12 +15208,13 @@
       <c r="Z77" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA77" s="2" t="s">
+      <c r="AA77" s="19"/>
+      <c r="AB77" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB77" s="2"/>
-    </row>
-    <row r="78" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC77" s="2"/>
+    </row>
+    <row r="78" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="5" t="s">
         <v>598</v>
       </c>
@@ -15161,12 +15273,13 @@
       <c r="Z78" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA78" s="2" t="s">
+      <c r="AA78" s="19"/>
+      <c r="AB78" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB78" s="2"/>
-    </row>
-    <row r="79" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC78" s="2"/>
+    </row>
+    <row r="79" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="5" t="s">
         <v>604</v>
       </c>
@@ -15225,12 +15338,13 @@
       <c r="Z79" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA79" s="2" t="s">
+      <c r="AA79" s="19"/>
+      <c r="AB79" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB79" s="2"/>
-    </row>
-    <row r="80" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC79" s="2"/>
+    </row>
+    <row r="80" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="5" t="s">
         <v>611</v>
       </c>
@@ -15289,12 +15403,13 @@
       <c r="Z80" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA80" s="2" t="s">
+      <c r="AA80" s="19"/>
+      <c r="AB80" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB80" s="2"/>
-    </row>
-    <row r="81" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC80" s="2"/>
+    </row>
+    <row r="81" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="5" t="s">
         <v>618</v>
       </c>
@@ -15353,12 +15468,13 @@
       <c r="Z81" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA81" s="2" t="s">
+      <c r="AA81" s="19"/>
+      <c r="AB81" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB81" s="2"/>
-    </row>
-    <row r="82" spans="1:28" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC81" s="2"/>
+    </row>
+    <row r="82" spans="1:29" ht="374.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="5" t="s">
         <v>626</v>
       </c>
@@ -15417,12 +15533,13 @@
       <c r="Z82" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA82" s="2" t="s">
+      <c r="AA82" s="19"/>
+      <c r="AB82" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB82" s="2"/>
-    </row>
-    <row r="83" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC82" s="2"/>
+    </row>
+    <row r="83" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="5" t="s">
         <v>633</v>
       </c>
@@ -15481,12 +15598,13 @@
       <c r="Z83" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA83" s="2" t="s">
+      <c r="AA83" s="19"/>
+      <c r="AB83" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB83" s="2"/>
-    </row>
-    <row r="84" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC83" s="2"/>
+    </row>
+    <row r="84" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="5" t="s">
         <v>640</v>
       </c>
@@ -15545,12 +15663,13 @@
       <c r="Z84" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA84" s="2" t="s">
+      <c r="AA84" s="19"/>
+      <c r="AB84" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB84" s="2"/>
-    </row>
-    <row r="85" spans="1:28" ht="288" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC84" s="2"/>
+    </row>
+    <row r="85" spans="1:29" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="5" t="s">
         <v>646</v>
       </c>
@@ -15609,12 +15728,13 @@
       <c r="Z85" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA85" s="2" t="s">
+      <c r="AA85" s="19"/>
+      <c r="AB85" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB85" s="2"/>
-    </row>
-    <row r="86" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC85" s="2"/>
+    </row>
+    <row r="86" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="7" t="s">
         <v>653</v>
       </c>
@@ -15673,12 +15793,13 @@
       <c r="Z86" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA86" s="2" t="s">
+      <c r="AA86" s="19"/>
+      <c r="AB86" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB86" s="2"/>
-    </row>
-    <row r="87" spans="1:28" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC86" s="2"/>
+    </row>
+    <row r="87" spans="1:29" ht="374.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="5" t="s">
         <v>660</v>
       </c>
@@ -15737,12 +15858,13 @@
       <c r="Z87" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA87" s="2" t="s">
+      <c r="AA87" s="19"/>
+      <c r="AB87" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB87" s="2"/>
-    </row>
-    <row r="88" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC87" s="2"/>
+    </row>
+    <row r="88" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="5" t="s">
         <v>667</v>
       </c>
@@ -15801,12 +15923,13 @@
       <c r="Z88" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA88" s="2" t="s">
+      <c r="AA88" s="19"/>
+      <c r="AB88" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB88" s="2"/>
-    </row>
-    <row r="89" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC88" s="2"/>
+    </row>
+    <row r="89" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="5" t="s">
         <v>674</v>
       </c>
@@ -15865,12 +15988,13 @@
       <c r="Z89" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA89" s="2" t="s">
+      <c r="AA89" s="19"/>
+      <c r="AB89" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB89" s="2"/>
-    </row>
-    <row r="90" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC89" s="2"/>
+    </row>
+    <row r="90" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="5" t="s">
         <v>681</v>
       </c>
@@ -15929,12 +16053,13 @@
       <c r="Z90" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA90" s="2" t="s">
+      <c r="AA90" s="19"/>
+      <c r="AB90" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB90" s="2"/>
-    </row>
-    <row r="91" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC90" s="2"/>
+    </row>
+    <row r="91" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="5" t="s">
         <v>688</v>
       </c>
@@ -15993,12 +16118,13 @@
       <c r="Z91" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA91" s="2" t="s">
+      <c r="AA91" s="19"/>
+      <c r="AB91" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB91" s="2"/>
-    </row>
-    <row r="92" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC91" s="2"/>
+    </row>
+    <row r="92" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="5" t="s">
         <v>695</v>
       </c>
@@ -16057,12 +16183,13 @@
       <c r="Z92" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA92" s="2" t="s">
+      <c r="AA92" s="19"/>
+      <c r="AB92" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB92" s="2"/>
-    </row>
-    <row r="93" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC92" s="2"/>
+    </row>
+    <row r="93" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="5" t="s">
         <v>701</v>
       </c>
@@ -16121,12 +16248,13 @@
       <c r="Z93" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA93" s="2" t="s">
+      <c r="AA93" s="19"/>
+      <c r="AB93" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB93" s="2"/>
-    </row>
-    <row r="94" spans="1:28" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC93" s="2"/>
+    </row>
+    <row r="94" spans="1:29" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="5" t="s">
         <v>707</v>
       </c>
@@ -16185,12 +16313,13 @@
       <c r="Z94" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA94" s="2" t="s">
+      <c r="AA94" s="19"/>
+      <c r="AB94" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB94" s="2"/>
-    </row>
-    <row r="95" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC94" s="2"/>
+    </row>
+    <row r="95" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="7" t="s">
         <v>713</v>
       </c>
@@ -16249,12 +16378,13 @@
       <c r="Z95" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA95" s="2" t="s">
+      <c r="AA95" s="19"/>
+      <c r="AB95" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB95" s="2"/>
-    </row>
-    <row r="96" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC95" s="2"/>
+    </row>
+    <row r="96" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="5" t="s">
         <v>720</v>
       </c>
@@ -16313,12 +16443,13 @@
       <c r="Z96" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA96" s="2" t="s">
+      <c r="AA96" s="19"/>
+      <c r="AB96" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB96" s="2"/>
-    </row>
-    <row r="97" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC96" s="2"/>
+    </row>
+    <row r="97" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="5" t="s">
         <v>727</v>
       </c>
@@ -16377,12 +16508,13 @@
       <c r="Z97" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA97" s="2" t="s">
+      <c r="AA97" s="19"/>
+      <c r="AB97" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB97" s="2"/>
-    </row>
-    <row r="98" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC97" s="2"/>
+    </row>
+    <row r="98" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="5" t="s">
         <v>734</v>
       </c>
@@ -16441,12 +16573,13 @@
       <c r="Z98" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA98" s="2" t="s">
+      <c r="AA98" s="19"/>
+      <c r="AB98" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB98" s="2"/>
-    </row>
-    <row r="99" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC98" s="2"/>
+    </row>
+    <row r="99" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="7" t="s">
         <v>741</v>
       </c>
@@ -16505,12 +16638,13 @@
       <c r="Z99" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA99" s="2" t="s">
+      <c r="AA99" s="19"/>
+      <c r="AB99" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB99" s="2"/>
-    </row>
-    <row r="100" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC99" s="2"/>
+    </row>
+    <row r="100" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="5" t="s">
         <v>749</v>
       </c>
@@ -16569,12 +16703,13 @@
       <c r="Z100" s="14" t="s">
         <v>1786</v>
       </c>
-      <c r="AA100" s="2" t="s">
+      <c r="AA100" s="19"/>
+      <c r="AB100" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB100" s="2"/>
-    </row>
-    <row r="101" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC100" s="2"/>
+    </row>
+    <row r="101" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="5" t="s">
         <v>756</v>
       </c>
@@ -16633,12 +16768,13 @@
       <c r="Z101" s="14" t="s">
         <v>1801</v>
       </c>
-      <c r="AA101" s="2" t="s">
+      <c r="AA101" s="19"/>
+      <c r="AB101" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB101" s="2"/>
-    </row>
-    <row r="102" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC101" s="2"/>
+    </row>
+    <row r="102" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="7" t="s">
         <v>765</v>
       </c>
@@ -16697,12 +16833,13 @@
       <c r="Z102" s="14" t="s">
         <v>1802</v>
       </c>
-      <c r="AA102" s="2" t="s">
+      <c r="AA102" s="19"/>
+      <c r="AB102" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB102" s="2"/>
-    </row>
-    <row r="103" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC102" s="2"/>
+    </row>
+    <row r="103" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="7" t="s">
         <v>774</v>
       </c>
@@ -16761,12 +16898,13 @@
       <c r="Z103" s="15" t="s">
         <v>1803</v>
       </c>
-      <c r="AA103" s="2" t="s">
+      <c r="AA103" s="20"/>
+      <c r="AB103" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB103" s="2"/>
-    </row>
-    <row r="104" spans="1:28" ht="259.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC103" s="2"/>
+    </row>
+    <row r="104" spans="1:29" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="7" t="s">
         <v>783</v>
       </c>
@@ -16825,12 +16963,13 @@
       <c r="Z104" s="15" t="s">
         <v>1803</v>
       </c>
-      <c r="AA104" s="2" t="s">
+      <c r="AA104" s="20"/>
+      <c r="AB104" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB104" s="2"/>
-    </row>
-    <row r="105" spans="1:28" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC104" s="2"/>
+    </row>
+    <row r="105" spans="1:29" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="7" t="s">
         <v>789</v>
       </c>
@@ -16889,12 +17028,13 @@
       <c r="Z105" s="15" t="s">
         <v>1803</v>
       </c>
-      <c r="AA105" s="2" t="s">
+      <c r="AA105" s="20"/>
+      <c r="AB105" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB105" s="2"/>
-    </row>
-    <row r="106" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC105" s="2"/>
+    </row>
+    <row r="106" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="7" t="s">
         <v>796</v>
       </c>
@@ -16953,12 +17093,13 @@
       <c r="Z106" s="14" t="s">
         <v>1804</v>
       </c>
-      <c r="AA106" s="2" t="s">
+      <c r="AA106" s="19"/>
+      <c r="AB106" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB106" s="2"/>
-    </row>
-    <row r="107" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC106" s="2"/>
+    </row>
+    <row r="107" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="7" t="s">
         <v>805</v>
       </c>
@@ -17017,12 +17158,13 @@
       <c r="Z107" s="14" t="s">
         <v>1804</v>
       </c>
-      <c r="AA107" s="2" t="s">
+      <c r="AA107" s="19"/>
+      <c r="AB107" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB107" s="2"/>
-    </row>
-    <row r="108" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC107" s="2"/>
+    </row>
+    <row r="108" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="7" t="s">
         <v>812</v>
       </c>
@@ -17081,12 +17223,13 @@
       <c r="Z108" s="14" t="s">
         <v>1804</v>
       </c>
-      <c r="AA108" s="2" t="s">
+      <c r="AA108" s="19"/>
+      <c r="AB108" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB108" s="2"/>
-    </row>
-    <row r="109" spans="1:28" ht="388.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC108" s="2"/>
+    </row>
+    <row r="109" spans="1:29" ht="388.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="7" t="s">
         <v>818</v>
       </c>
@@ -17145,12 +17288,13 @@
       <c r="Z109" s="14" t="s">
         <v>1805</v>
       </c>
-      <c r="AA109" s="2" t="s">
+      <c r="AA109" s="19"/>
+      <c r="AB109" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB109" s="2"/>
-    </row>
-    <row r="110" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC109" s="2"/>
+    </row>
+    <row r="110" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="5" t="s">
         <v>827</v>
       </c>
@@ -17209,12 +17353,13 @@
       <c r="Z110" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA110" s="2" t="s">
+      <c r="AA110" s="19"/>
+      <c r="AB110" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB110" s="2"/>
-    </row>
-    <row r="111" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC110" s="2"/>
+    </row>
+    <row r="111" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="5" t="s">
         <v>836</v>
       </c>
@@ -17273,12 +17418,13 @@
       <c r="Z111" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA111" s="2" t="s">
+      <c r="AA111" s="19"/>
+      <c r="AB111" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB111" s="2"/>
-    </row>
-    <row r="112" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC111" s="2"/>
+    </row>
+    <row r="112" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="5" t="s">
         <v>842</v>
       </c>
@@ -17337,12 +17483,13 @@
       <c r="Z112" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA112" s="2" t="s">
+      <c r="AA112" s="19"/>
+      <c r="AB112" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB112" s="2"/>
-    </row>
-    <row r="113" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC112" s="2"/>
+    </row>
+    <row r="113" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="5" t="s">
         <v>848</v>
       </c>
@@ -17401,12 +17548,13 @@
       <c r="Z113" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA113" s="2" t="s">
+      <c r="AA113" s="19"/>
+      <c r="AB113" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB113" s="2"/>
-    </row>
-    <row r="114" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC113" s="2"/>
+    </row>
+    <row r="114" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="5" t="s">
         <v>854</v>
       </c>
@@ -17465,12 +17613,13 @@
       <c r="Z114" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA114" s="2" t="s">
+      <c r="AA114" s="19"/>
+      <c r="AB114" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB114" s="2"/>
-    </row>
-    <row r="115" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC114" s="2"/>
+    </row>
+    <row r="115" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="5" t="s">
         <v>863</v>
       </c>
@@ -17529,12 +17678,13 @@
       <c r="Z115" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA115" s="2" t="s">
+      <c r="AA115" s="19"/>
+      <c r="AB115" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB115" s="2"/>
-    </row>
-    <row r="116" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC115" s="2"/>
+    </row>
+    <row r="116" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="5" t="s">
         <v>869</v>
       </c>
@@ -17593,12 +17743,13 @@
       <c r="Z116" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA116" s="2" t="s">
+      <c r="AA116" s="19"/>
+      <c r="AB116" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB116" s="2"/>
-    </row>
-    <row r="117" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC116" s="2"/>
+    </row>
+    <row r="117" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="5" t="s">
         <v>875</v>
       </c>
@@ -17657,12 +17808,13 @@
       <c r="Z117" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA117" s="2" t="s">
+      <c r="AA117" s="19"/>
+      <c r="AB117" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB117" s="2"/>
-    </row>
-    <row r="118" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC117" s="2"/>
+    </row>
+    <row r="118" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="5" t="s">
         <v>881</v>
       </c>
@@ -17721,12 +17873,13 @@
       <c r="Z118" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA118" s="2" t="s">
+      <c r="AA118" s="19"/>
+      <c r="AB118" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB118" s="2"/>
-    </row>
-    <row r="119" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC118" s="2"/>
+    </row>
+    <row r="119" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="5" t="s">
         <v>887</v>
       </c>
@@ -17785,12 +17938,13 @@
       <c r="Z119" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA119" s="2" t="s">
+      <c r="AA119" s="19"/>
+      <c r="AB119" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB119" s="2"/>
-    </row>
-    <row r="120" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC119" s="2"/>
+    </row>
+    <row r="120" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="5" t="s">
         <v>893</v>
       </c>
@@ -17849,12 +18003,13 @@
       <c r="Z120" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA120" s="2" t="s">
+      <c r="AA120" s="19"/>
+      <c r="AB120" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB120" s="2"/>
-    </row>
-    <row r="121" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC120" s="2"/>
+    </row>
+    <row r="121" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="5" t="s">
         <v>899</v>
       </c>
@@ -17913,12 +18068,13 @@
       <c r="Z121" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA121" s="2" t="s">
+      <c r="AA121" s="19"/>
+      <c r="AB121" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB121" s="2"/>
-    </row>
-    <row r="122" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC121" s="2"/>
+    </row>
+    <row r="122" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="5" t="s">
         <v>905</v>
       </c>
@@ -17977,12 +18133,13 @@
       <c r="Z122" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA122" s="2" t="s">
+      <c r="AA122" s="19"/>
+      <c r="AB122" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB122" s="2"/>
-    </row>
-    <row r="123" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC122" s="2"/>
+    </row>
+    <row r="123" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="5" t="s">
         <v>911</v>
       </c>
@@ -18041,12 +18198,13 @@
       <c r="Z123" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA123" s="2" t="s">
+      <c r="AA123" s="19"/>
+      <c r="AB123" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB123" s="2"/>
-    </row>
-    <row r="124" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC123" s="2"/>
+    </row>
+    <row r="124" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="5" t="s">
         <v>919</v>
       </c>
@@ -18105,12 +18263,13 @@
       <c r="Z124" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA124" s="2" t="s">
+      <c r="AA124" s="19"/>
+      <c r="AB124" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB124" s="2"/>
-    </row>
-    <row r="125" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC124" s="2"/>
+    </row>
+    <row r="125" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="5" t="s">
         <v>925</v>
       </c>
@@ -18169,12 +18328,13 @@
       <c r="Z125" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA125" s="2" t="s">
+      <c r="AA125" s="19"/>
+      <c r="AB125" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB125" s="2"/>
-    </row>
-    <row r="126" spans="1:28" ht="331.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC125" s="2"/>
+    </row>
+    <row r="126" spans="1:29" ht="331.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="5" t="s">
         <v>931</v>
       </c>
@@ -18233,12 +18393,13 @@
       <c r="Z126" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA126" s="2" t="s">
+      <c r="AA126" s="19"/>
+      <c r="AB126" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB126" s="2"/>
-    </row>
-    <row r="127" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC126" s="2"/>
+    </row>
+    <row r="127" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="5" t="s">
         <v>937</v>
       </c>
@@ -18297,12 +18458,13 @@
       <c r="Z127" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA127" s="2" t="s">
+      <c r="AA127" s="19"/>
+      <c r="AB127" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB127" s="2"/>
-    </row>
-    <row r="128" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC127" s="2"/>
+    </row>
+    <row r="128" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="5" t="s">
         <v>943</v>
       </c>
@@ -18361,12 +18523,13 @@
       <c r="Z128" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA128" s="2" t="s">
+      <c r="AA128" s="19"/>
+      <c r="AB128" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB128" s="2"/>
-    </row>
-    <row r="129" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC128" s="2"/>
+    </row>
+    <row r="129" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="5" t="s">
         <v>949</v>
       </c>
@@ -18425,12 +18588,13 @@
       <c r="Z129" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA129" s="2" t="s">
+      <c r="AA129" s="19"/>
+      <c r="AB129" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB129" s="2"/>
-    </row>
-    <row r="130" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC129" s="2"/>
+    </row>
+    <row r="130" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="5" t="s">
         <v>957</v>
       </c>
@@ -18489,12 +18653,13 @@
       <c r="Z130" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA130" s="2" t="s">
+      <c r="AA130" s="19"/>
+      <c r="AB130" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB130" s="2"/>
-    </row>
-    <row r="131" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC130" s="2"/>
+    </row>
+    <row r="131" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="5" t="s">
         <v>963</v>
       </c>
@@ -18553,12 +18718,13 @@
       <c r="Z131" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA131" s="2" t="s">
+      <c r="AA131" s="19"/>
+      <c r="AB131" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB131" s="2"/>
-    </row>
-    <row r="132" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC131" s="2"/>
+    </row>
+    <row r="132" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="5" t="s">
         <v>969</v>
       </c>
@@ -18617,12 +18783,13 @@
       <c r="Z132" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA132" s="2" t="s">
+      <c r="AA132" s="19"/>
+      <c r="AB132" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB132" s="2"/>
-    </row>
-    <row r="133" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC132" s="2"/>
+    </row>
+    <row r="133" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="5" t="s">
         <v>975</v>
       </c>
@@ -18681,12 +18848,13 @@
       <c r="Z133" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA133" s="2" t="s">
+      <c r="AA133" s="19"/>
+      <c r="AB133" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB133" s="2"/>
-    </row>
-    <row r="134" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC133" s="2"/>
+    </row>
+    <row r="134" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="5" t="s">
         <v>983</v>
       </c>
@@ -18745,12 +18913,13 @@
       <c r="Z134" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA134" s="2" t="s">
+      <c r="AA134" s="19"/>
+      <c r="AB134" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB134" s="2"/>
-    </row>
-    <row r="135" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC134" s="2"/>
+    </row>
+    <row r="135" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="5" t="s">
         <v>989</v>
       </c>
@@ -18809,12 +18978,13 @@
       <c r="Z135" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA135" s="2" t="s">
+      <c r="AA135" s="19"/>
+      <c r="AB135" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB135" s="2"/>
-    </row>
-    <row r="136" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC135" s="2"/>
+    </row>
+    <row r="136" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="5" t="s">
         <v>995</v>
       </c>
@@ -18873,12 +19043,13 @@
       <c r="Z136" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA136" s="2" t="s">
+      <c r="AA136" s="19"/>
+      <c r="AB136" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB136" s="2"/>
-    </row>
-    <row r="137" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC136" s="2"/>
+    </row>
+    <row r="137" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="5" t="s">
         <v>1004</v>
       </c>
@@ -18937,12 +19108,13 @@
       <c r="Z137" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA137" s="2" t="s">
+      <c r="AA137" s="19"/>
+      <c r="AB137" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB137" s="2"/>
-    </row>
-    <row r="138" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC137" s="2"/>
+    </row>
+    <row r="138" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="5" t="s">
         <v>1010</v>
       </c>
@@ -19001,12 +19173,13 @@
       <c r="Z138" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA138" s="2" t="s">
+      <c r="AA138" s="19"/>
+      <c r="AB138" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB138" s="2"/>
-    </row>
-    <row r="139" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC138" s="2"/>
+    </row>
+    <row r="139" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="5" t="s">
         <v>1016</v>
       </c>
@@ -19065,12 +19238,13 @@
       <c r="Z139" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA139" s="2" t="s">
+      <c r="AA139" s="19"/>
+      <c r="AB139" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB139" s="2"/>
-    </row>
-    <row r="140" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC139" s="2"/>
+    </row>
+    <row r="140" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="5" t="s">
         <v>1022</v>
       </c>
@@ -19129,12 +19303,13 @@
       <c r="Z140" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA140" s="2" t="s">
+      <c r="AA140" s="19"/>
+      <c r="AB140" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB140" s="2"/>
-    </row>
-    <row r="141" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC140" s="2"/>
+    </row>
+    <row r="141" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="5" t="s">
         <v>1028</v>
       </c>
@@ -19193,12 +19368,13 @@
       <c r="Z141" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA141" s="2" t="s">
+      <c r="AA141" s="19"/>
+      <c r="AB141" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB141" s="2"/>
-    </row>
-    <row r="142" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC141" s="2"/>
+    </row>
+    <row r="142" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="5" t="s">
         <v>1037</v>
       </c>
@@ -19257,12 +19433,13 @@
       <c r="Z142" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA142" s="2" t="s">
+      <c r="AA142" s="19"/>
+      <c r="AB142" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB142" s="2"/>
-    </row>
-    <row r="143" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC142" s="2"/>
+    </row>
+    <row r="143" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="5" t="s">
         <v>1043</v>
       </c>
@@ -19321,12 +19498,13 @@
       <c r="Z143" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA143" s="2" t="s">
+      <c r="AA143" s="19"/>
+      <c r="AB143" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB143" s="2"/>
-    </row>
-    <row r="144" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC143" s="2"/>
+    </row>
+    <row r="144" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="5" t="s">
         <v>1049</v>
       </c>
@@ -19385,12 +19563,13 @@
       <c r="Z144" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA144" s="2" t="s">
+      <c r="AA144" s="19"/>
+      <c r="AB144" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB144" s="2"/>
-    </row>
-    <row r="145" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC144" s="2"/>
+    </row>
+    <row r="145" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="5" t="s">
         <v>1055</v>
       </c>
@@ -19449,12 +19628,13 @@
       <c r="Z145" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA145" s="2" t="s">
+      <c r="AA145" s="19"/>
+      <c r="AB145" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB145" s="2"/>
-    </row>
-    <row r="146" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC145" s="2"/>
+    </row>
+    <row r="146" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="5" t="s">
         <v>1061</v>
       </c>
@@ -19513,12 +19693,13 @@
       <c r="Z146" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA146" s="2" t="s">
+      <c r="AA146" s="19"/>
+      <c r="AB146" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB146" s="2"/>
-    </row>
-    <row r="147" spans="1:28" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC146" s="2"/>
+    </row>
+    <row r="147" spans="1:29" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="5" t="s">
         <v>1067</v>
       </c>
@@ -19577,12 +19758,13 @@
       <c r="Z147" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA147" s="2" t="s">
+      <c r="AA147" s="19"/>
+      <c r="AB147" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB147" s="2"/>
-    </row>
-    <row r="148" spans="1:28" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC147" s="2"/>
+    </row>
+    <row r="148" spans="1:29" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="5" t="s">
         <v>1075</v>
       </c>
@@ -19641,12 +19823,13 @@
       <c r="Z148" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA148" s="2" t="s">
+      <c r="AA148" s="19"/>
+      <c r="AB148" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB148" s="2"/>
-    </row>
-    <row r="149" spans="1:28" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC148" s="2"/>
+    </row>
+    <row r="149" spans="1:29" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="5" t="s">
         <v>1081</v>
       </c>
@@ -19705,12 +19888,13 @@
       <c r="Z149" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA149" s="2" t="s">
+      <c r="AA149" s="19"/>
+      <c r="AB149" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB149" s="2"/>
-    </row>
-    <row r="150" spans="1:28" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC149" s="2"/>
+    </row>
+    <row r="150" spans="1:29" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="7" t="s">
         <v>1088</v>
       </c>
@@ -19769,12 +19953,13 @@
       <c r="Z150" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA150" s="2" t="s">
+      <c r="AA150" s="19"/>
+      <c r="AB150" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB150" s="2"/>
-    </row>
-    <row r="151" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC150" s="2"/>
+    </row>
+    <row r="151" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="5" t="s">
         <v>1094</v>
       </c>
@@ -19833,12 +20018,13 @@
       <c r="Z151" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA151" s="2" t="s">
+      <c r="AA151" s="19"/>
+      <c r="AB151" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB151" s="2"/>
-    </row>
-    <row r="152" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC151" s="2"/>
+    </row>
+    <row r="152" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="5" t="s">
         <v>1101</v>
       </c>
@@ -19897,12 +20083,13 @@
       <c r="Z152" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA152" s="2" t="s">
+      <c r="AA152" s="19"/>
+      <c r="AB152" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB152" s="2"/>
-    </row>
-    <row r="153" spans="1:28" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC152" s="2"/>
+    </row>
+    <row r="153" spans="1:29" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="5" t="s">
         <v>1108</v>
       </c>
@@ -19961,12 +20148,13 @@
       <c r="Z153" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA153" s="2" t="s">
+      <c r="AA153" s="19"/>
+      <c r="AB153" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB153" s="2"/>
-    </row>
-    <row r="154" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC153" s="2"/>
+    </row>
+    <row r="154" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="5" t="s">
         <v>1116</v>
       </c>
@@ -20025,12 +20213,13 @@
       <c r="Z154" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA154" s="2" t="s">
+      <c r="AA154" s="19"/>
+      <c r="AB154" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB154" s="2"/>
-    </row>
-    <row r="155" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC154" s="2"/>
+    </row>
+    <row r="155" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="5" t="s">
         <v>1124</v>
       </c>
@@ -20089,12 +20278,13 @@
       <c r="Z155" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA155" s="2" t="s">
+      <c r="AA155" s="19"/>
+      <c r="AB155" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB155" s="2"/>
-    </row>
-    <row r="156" spans="1:28" ht="259.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC155" s="2"/>
+    </row>
+    <row r="156" spans="1:29" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="5" t="s">
         <v>1130</v>
       </c>
@@ -20153,12 +20343,13 @@
       <c r="Z156" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA156" s="2" t="s">
+      <c r="AA156" s="19"/>
+      <c r="AB156" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB156" s="2"/>
-    </row>
-    <row r="157" spans="1:28" ht="259.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC156" s="2"/>
+    </row>
+    <row r="157" spans="1:29" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="5" t="s">
         <v>1136</v>
       </c>
@@ -20217,12 +20408,13 @@
       <c r="Z157" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA157" s="2" t="s">
+      <c r="AA157" s="19"/>
+      <c r="AB157" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB157" s="2"/>
-    </row>
-    <row r="158" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC157" s="2"/>
+    </row>
+    <row r="158" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="5" t="s">
         <v>1142</v>
       </c>
@@ -20281,12 +20473,13 @@
       <c r="Z158" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA158" s="2" t="s">
+      <c r="AA158" s="19"/>
+      <c r="AB158" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB158" s="2"/>
-    </row>
-    <row r="159" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC158" s="2"/>
+    </row>
+    <row r="159" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="5" t="s">
         <v>1148</v>
       </c>
@@ -20345,12 +20538,13 @@
       <c r="Z159" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA159" s="2" t="s">
+      <c r="AA159" s="19"/>
+      <c r="AB159" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB159" s="2"/>
-    </row>
-    <row r="160" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC159" s="2"/>
+    </row>
+    <row r="160" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="5" t="s">
         <v>1157</v>
       </c>
@@ -20409,12 +20603,13 @@
       <c r="Z160" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA160" s="2" t="s">
+      <c r="AA160" s="19"/>
+      <c r="AB160" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB160" s="2"/>
-    </row>
-    <row r="161" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC160" s="2"/>
+    </row>
+    <row r="161" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="5" t="s">
         <v>1165</v>
       </c>
@@ -20473,12 +20668,13 @@
       <c r="Z161" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA161" s="2" t="s">
+      <c r="AA161" s="19"/>
+      <c r="AB161" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB161" s="2"/>
-    </row>
-    <row r="162" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC161" s="2"/>
+    </row>
+    <row r="162" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="5" t="s">
         <v>1171</v>
       </c>
@@ -20537,12 +20733,13 @@
       <c r="Z162" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA162" s="2" t="s">
+      <c r="AA162" s="19"/>
+      <c r="AB162" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB162" s="2"/>
-    </row>
-    <row r="163" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC162" s="2"/>
+    </row>
+    <row r="163" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="5" t="s">
         <v>1177</v>
       </c>
@@ -20601,12 +20798,13 @@
       <c r="Z163" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA163" s="2" t="s">
+      <c r="AA163" s="19"/>
+      <c r="AB163" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB163" s="2"/>
-    </row>
-    <row r="164" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC163" s="2"/>
+    </row>
+    <row r="164" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="5" t="s">
         <v>1183</v>
       </c>
@@ -20665,12 +20863,13 @@
       <c r="Z164" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA164" s="2" t="s">
+      <c r="AA164" s="19"/>
+      <c r="AB164" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB164" s="2"/>
-    </row>
-    <row r="165" spans="1:28" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC164" s="2"/>
+    </row>
+    <row r="165" spans="1:29" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="5" t="s">
         <v>1189</v>
       </c>
@@ -20729,12 +20928,13 @@
       <c r="Z165" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA165" s="2" t="s">
+      <c r="AA165" s="19"/>
+      <c r="AB165" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB165" s="2"/>
-    </row>
-    <row r="166" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC165" s="2"/>
+    </row>
+    <row r="166" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="5" t="s">
         <v>1196</v>
       </c>
@@ -20793,12 +20993,13 @@
       <c r="Z166" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA166" s="2" t="s">
+      <c r="AA166" s="19"/>
+      <c r="AB166" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB166" s="2"/>
-    </row>
-    <row r="167" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC166" s="2"/>
+    </row>
+    <row r="167" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="5" t="s">
         <v>1203</v>
       </c>
@@ -20857,12 +21058,13 @@
       <c r="Z167" s="14" t="s">
         <v>1807</v>
       </c>
-      <c r="AA167" s="2" t="s">
+      <c r="AA167" s="19"/>
+      <c r="AB167" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB167" s="2"/>
-    </row>
-    <row r="168" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC167" s="2"/>
+    </row>
+    <row r="168" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="5" t="s">
         <v>1211</v>
       </c>
@@ -20921,12 +21123,13 @@
       <c r="Z168" s="14" t="s">
         <v>1807</v>
       </c>
-      <c r="AA168" s="2" t="s">
+      <c r="AA168" s="19"/>
+      <c r="AB168" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB168" s="2"/>
-    </row>
-    <row r="169" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC168" s="2"/>
+    </row>
+    <row r="169" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="7" t="s">
         <v>1218</v>
       </c>
@@ -20985,12 +21188,13 @@
       <c r="Z169" s="14" t="s">
         <v>1808</v>
       </c>
-      <c r="AA169" s="2" t="s">
+      <c r="AA169" s="19"/>
+      <c r="AB169" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB169" s="2"/>
-    </row>
-    <row r="170" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC169" s="2"/>
+    </row>
+    <row r="170" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="5" t="s">
         <v>1227</v>
       </c>
@@ -21049,12 +21253,13 @@
       <c r="Z170" s="14" t="s">
         <v>1786</v>
       </c>
-      <c r="AA170" s="2" t="s">
+      <c r="AA170" s="19"/>
+      <c r="AB170" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB170" s="2"/>
-    </row>
-    <row r="171" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC170" s="2"/>
+    </row>
+    <row r="171" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="7" t="s">
         <v>1236</v>
       </c>
@@ -21113,12 +21318,13 @@
       <c r="Z171" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA171" s="2" t="s">
+      <c r="AA171" s="19"/>
+      <c r="AB171" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB171" s="2"/>
-    </row>
-    <row r="172" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC171" s="2"/>
+    </row>
+    <row r="172" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="7" t="s">
         <v>1243</v>
       </c>
@@ -21177,12 +21383,13 @@
       <c r="Z172" s="14" t="s">
         <v>1809</v>
       </c>
-      <c r="AA172" s="2" t="s">
+      <c r="AA172" s="19"/>
+      <c r="AB172" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB172" s="2"/>
-    </row>
-    <row r="173" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC172" s="2"/>
+    </row>
+    <row r="173" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="7" t="s">
         <v>1252</v>
       </c>
@@ -21241,12 +21448,13 @@
       <c r="Z173" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="AA173" s="2" t="s">
+      <c r="AA173" s="19"/>
+      <c r="AB173" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB173" s="2"/>
-    </row>
-    <row r="174" spans="1:28" ht="259.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC173" s="2"/>
+    </row>
+    <row r="174" spans="1:29" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="7" t="s">
         <v>1256</v>
       </c>
@@ -21305,12 +21513,13 @@
       <c r="Z174" s="14" t="s">
         <v>1813</v>
       </c>
-      <c r="AA174" s="2" t="s">
+      <c r="AA174" s="19"/>
+      <c r="AB174" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB174" s="2"/>
-    </row>
-    <row r="175" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC174" s="2"/>
+    </row>
+    <row r="175" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="7" t="s">
         <v>1265</v>
       </c>
@@ -21369,12 +21578,13 @@
       <c r="Z175" s="14" t="s">
         <v>1813</v>
       </c>
-      <c r="AA175" s="2" t="s">
+      <c r="AA175" s="19"/>
+      <c r="AB175" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB175" s="2"/>
-    </row>
-    <row r="176" spans="1:28" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC175" s="2"/>
+    </row>
+    <row r="176" spans="1:29" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="7" t="s">
         <v>1271</v>
       </c>
@@ -21433,12 +21643,13 @@
       <c r="Z176" s="14" t="s">
         <v>1813</v>
       </c>
-      <c r="AA176" s="2" t="s">
+      <c r="AA176" s="19"/>
+      <c r="AB176" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB176" s="2"/>
-    </row>
-    <row r="177" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC176" s="2"/>
+    </row>
+    <row r="177" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="7" t="s">
         <v>1276</v>
       </c>
@@ -21497,12 +21708,13 @@
       <c r="Z177" s="14" t="s">
         <v>1814</v>
       </c>
-      <c r="AA177" s="2" t="s">
+      <c r="AA177" s="19"/>
+      <c r="AB177" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB177" s="2"/>
-    </row>
-    <row r="178" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC177" s="2"/>
+    </row>
+    <row r="178" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="7" t="s">
         <v>1285</v>
       </c>
@@ -21561,12 +21773,13 @@
       <c r="Z178" s="14" t="s">
         <v>1814</v>
       </c>
-      <c r="AA178" s="2" t="s">
+      <c r="AA178" s="19"/>
+      <c r="AB178" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB178" s="2"/>
-    </row>
-    <row r="179" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC178" s="2"/>
+    </row>
+    <row r="179" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="7" t="s">
         <v>1292</v>
       </c>
@@ -21625,12 +21838,13 @@
       <c r="Z179" s="14" t="s">
         <v>1809</v>
       </c>
-      <c r="AA179" s="2" t="s">
+      <c r="AA179" s="19"/>
+      <c r="AB179" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB179" s="2"/>
-    </row>
-    <row r="180" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC179" s="2"/>
+    </row>
+    <row r="180" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="5" t="s">
         <v>1299</v>
       </c>
@@ -21689,12 +21903,13 @@
       <c r="Z180" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA180" s="2" t="s">
+      <c r="AA180" s="19"/>
+      <c r="AB180" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB180" s="2"/>
-    </row>
-    <row r="181" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC180" s="2"/>
+    </row>
+    <row r="181" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="7" t="s">
         <v>1305</v>
       </c>
@@ -21753,12 +21968,13 @@
       <c r="Z181" s="14" t="s">
         <v>1815</v>
       </c>
-      <c r="AA181" s="2" t="s">
+      <c r="AA181" s="19"/>
+      <c r="AB181" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB181" s="2"/>
-    </row>
-    <row r="182" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC181" s="2"/>
+    </row>
+    <row r="182" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="5" t="s">
         <v>1311</v>
       </c>
@@ -21817,12 +22033,13 @@
       <c r="Z182" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA182" s="2" t="s">
+      <c r="AA182" s="19"/>
+      <c r="AB182" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB182" s="2"/>
-    </row>
-    <row r="183" spans="1:28" ht="288" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC182" s="2"/>
+    </row>
+    <row r="183" spans="1:29" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="5" t="s">
         <v>1317</v>
       </c>
@@ -21881,12 +22098,13 @@
       <c r="Z183" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA183" s="2" t="s">
+      <c r="AA183" s="19"/>
+      <c r="AB183" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB183" s="2"/>
-    </row>
-    <row r="184" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC183" s="2"/>
+    </row>
+    <row r="184" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="5" t="s">
         <v>1324</v>
       </c>
@@ -21945,12 +22163,13 @@
       <c r="Z184" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA184" s="2" t="s">
+      <c r="AA184" s="19"/>
+      <c r="AB184" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB184" s="2"/>
-    </row>
-    <row r="185" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC184" s="2"/>
+    </row>
+    <row r="185" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="5" t="s">
         <v>1331</v>
       </c>
@@ -22009,12 +22228,13 @@
       <c r="Z185" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA185" s="2" t="s">
+      <c r="AA185" s="19"/>
+      <c r="AB185" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB185" s="2"/>
-    </row>
-    <row r="186" spans="1:28" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC185" s="2"/>
+    </row>
+    <row r="186" spans="1:29" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="5" t="s">
         <v>1337</v>
       </c>
@@ -22073,12 +22293,13 @@
       <c r="Z186" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA186" s="2" t="s">
+      <c r="AA186" s="19"/>
+      <c r="AB186" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB186" s="2"/>
-    </row>
-    <row r="187" spans="1:28" ht="259.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC186" s="2"/>
+    </row>
+    <row r="187" spans="1:29" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="7" t="s">
         <v>1346</v>
       </c>
@@ -22137,12 +22358,13 @@
       <c r="Z187" s="14" t="s">
         <v>1813</v>
       </c>
-      <c r="AA187" s="2" t="s">
+      <c r="AA187" s="19"/>
+      <c r="AB187" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB187" s="2"/>
-    </row>
-    <row r="188" spans="1:28" ht="288" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC187" s="2"/>
+    </row>
+    <row r="188" spans="1:29" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="5" t="s">
         <v>1352</v>
       </c>
@@ -22201,12 +22423,13 @@
       <c r="Z188" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA188" s="2" t="s">
+      <c r="AA188" s="19"/>
+      <c r="AB188" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB188" s="2"/>
-    </row>
-    <row r="189" spans="1:28" ht="288" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC188" s="2"/>
+    </row>
+    <row r="189" spans="1:29" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="5" t="s">
         <v>1359</v>
       </c>
@@ -22265,12 +22488,13 @@
       <c r="Z189" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA189" s="2" t="s">
+      <c r="AA189" s="19"/>
+      <c r="AB189" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB189" s="2"/>
-    </row>
-    <row r="190" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC189" s="2"/>
+    </row>
+    <row r="190" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="5" t="s">
         <v>1366</v>
       </c>
@@ -22329,12 +22553,13 @@
       <c r="Z190" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA190" s="2" t="s">
+      <c r="AA190" s="19"/>
+      <c r="AB190" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB190" s="2"/>
-    </row>
-    <row r="191" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC190" s="2"/>
+    </row>
+    <row r="191" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="5" t="s">
         <v>1373</v>
       </c>
@@ -22393,12 +22618,13 @@
       <c r="Z191" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA191" s="2" t="s">
+      <c r="AA191" s="19"/>
+      <c r="AB191" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB191" s="2"/>
-    </row>
-    <row r="192" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC191" s="2"/>
+    </row>
+    <row r="192" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="5" t="s">
         <v>1380</v>
       </c>
@@ -22457,12 +22683,13 @@
       <c r="Z192" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA192" s="2" t="s">
+      <c r="AA192" s="19"/>
+      <c r="AB192" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB192" s="2"/>
-    </row>
-    <row r="193" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC192" s="2"/>
+    </row>
+    <row r="193" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="5" t="s">
         <v>1387</v>
       </c>
@@ -22521,12 +22748,13 @@
       <c r="Z193" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA193" s="2" t="s">
+      <c r="AA193" s="19"/>
+      <c r="AB193" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB193" s="2"/>
-    </row>
-    <row r="194" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC193" s="2"/>
+    </row>
+    <row r="194" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="5" t="s">
         <v>1394</v>
       </c>
@@ -22585,12 +22813,13 @@
       <c r="Z194" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA194" s="2" t="s">
+      <c r="AA194" s="19"/>
+      <c r="AB194" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB194" s="2"/>
-    </row>
-    <row r="195" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC194" s="2"/>
+    </row>
+    <row r="195" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="7" t="s">
         <v>1401</v>
       </c>
@@ -22649,12 +22878,13 @@
       <c r="Z195" s="14" t="s">
         <v>1816</v>
       </c>
-      <c r="AA195" s="2" t="s">
+      <c r="AA195" s="19"/>
+      <c r="AB195" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB195" s="2"/>
-    </row>
-    <row r="196" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC195" s="2"/>
+    </row>
+    <row r="196" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="5" t="s">
         <v>1410</v>
       </c>
@@ -22713,12 +22943,13 @@
       <c r="Z196" s="14" t="s">
         <v>1817</v>
       </c>
-      <c r="AA196" s="2" t="s">
+      <c r="AA196" s="19"/>
+      <c r="AB196" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB196" s="2"/>
-    </row>
-    <row r="197" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC196" s="2"/>
+    </row>
+    <row r="197" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="5" t="s">
         <v>1419</v>
       </c>
@@ -22777,12 +23008,13 @@
       <c r="Z197" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA197" s="2" t="s">
+      <c r="AA197" s="19"/>
+      <c r="AB197" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB197" s="2"/>
-    </row>
-    <row r="198" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC197" s="2"/>
+    </row>
+    <row r="198" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="5" t="s">
         <v>1426</v>
       </c>
@@ -22841,12 +23073,13 @@
       <c r="Z198" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA198" s="2" t="s">
+      <c r="AA198" s="19"/>
+      <c r="AB198" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB198" s="2"/>
-    </row>
-    <row r="199" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC198" s="2"/>
+    </row>
+    <row r="199" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="5" t="s">
         <v>1433</v>
       </c>
@@ -22905,12 +23138,13 @@
       <c r="Z199" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA199" s="2" t="s">
+      <c r="AA199" s="19"/>
+      <c r="AB199" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB199" s="2"/>
-    </row>
-    <row r="200" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC199" s="2"/>
+    </row>
+    <row r="200" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="5" t="s">
         <v>1440</v>
       </c>
@@ -22969,12 +23203,13 @@
       <c r="Z200" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA200" s="2" t="s">
+      <c r="AA200" s="19"/>
+      <c r="AB200" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB200" s="2"/>
-    </row>
-    <row r="201" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC200" s="2"/>
+    </row>
+    <row r="201" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="5" t="s">
         <v>1447</v>
       </c>
@@ -23033,12 +23268,13 @@
       <c r="Z201" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA201" s="2" t="s">
+      <c r="AA201" s="19"/>
+      <c r="AB201" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB201" s="2"/>
-    </row>
-    <row r="202" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC201" s="2"/>
+    </row>
+    <row r="202" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="5" t="s">
         <v>1454</v>
       </c>
@@ -23097,12 +23333,13 @@
       <c r="Z202" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA202" s="2" t="s">
+      <c r="AA202" s="19"/>
+      <c r="AB202" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB202" s="2"/>
-    </row>
-    <row r="203" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC202" s="2"/>
+    </row>
+    <row r="203" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="5" t="s">
         <v>1461</v>
       </c>
@@ -23161,12 +23398,13 @@
       <c r="Z203" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA203" s="2" t="s">
+      <c r="AA203" s="19"/>
+      <c r="AB203" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB203" s="2"/>
-    </row>
-    <row r="204" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC203" s="2"/>
+    </row>
+    <row r="204" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="5" t="s">
         <v>1467</v>
       </c>
@@ -23225,12 +23463,13 @@
       <c r="Z204" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA204" s="2" t="s">
+      <c r="AA204" s="19"/>
+      <c r="AB204" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB204" s="2"/>
-    </row>
-    <row r="205" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC204" s="2"/>
+    </row>
+    <row r="205" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="5" t="s">
         <v>1474</v>
       </c>
@@ -23289,12 +23528,13 @@
       <c r="Z205" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA205" s="2" t="s">
+      <c r="AA205" s="19"/>
+      <c r="AB205" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB205" s="2"/>
-    </row>
-    <row r="206" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC205" s="2"/>
+    </row>
+    <row r="206" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="5" t="s">
         <v>1481</v>
       </c>
@@ -23353,12 +23593,13 @@
       <c r="Z206" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA206" s="2" t="s">
+      <c r="AA206" s="19"/>
+      <c r="AB206" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB206" s="2"/>
-    </row>
-    <row r="207" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC206" s="2"/>
+    </row>
+    <row r="207" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="5" t="s">
         <v>1488</v>
       </c>
@@ -23417,12 +23658,13 @@
       <c r="Z207" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA207" s="2" t="s">
+      <c r="AA207" s="19"/>
+      <c r="AB207" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB207" s="2"/>
-    </row>
-    <row r="208" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC207" s="2"/>
+    </row>
+    <row r="208" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="5" t="s">
         <v>1494</v>
       </c>
@@ -23481,12 +23723,13 @@
       <c r="Z208" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA208" s="2" t="s">
+      <c r="AA208" s="19"/>
+      <c r="AB208" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB208" s="2"/>
-    </row>
-    <row r="209" spans="1:28" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC208" s="2"/>
+    </row>
+    <row r="209" spans="1:29" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="5" t="s">
         <v>1501</v>
       </c>
@@ -23545,12 +23788,13 @@
       <c r="Z209" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA209" s="2" t="s">
+      <c r="AA209" s="19"/>
+      <c r="AB209" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB209" s="2"/>
-    </row>
-    <row r="210" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC209" s="2"/>
+    </row>
+    <row r="210" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="5" t="s">
         <v>1508</v>
       </c>
@@ -23609,12 +23853,13 @@
       <c r="Z210" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA210" s="2" t="s">
+      <c r="AA210" s="19"/>
+      <c r="AB210" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB210" s="2"/>
-    </row>
-    <row r="211" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC210" s="2"/>
+    </row>
+    <row r="211" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="5" t="s">
         <v>1515</v>
       </c>
@@ -23673,12 +23918,13 @@
       <c r="Z211" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA211" s="2" t="s">
+      <c r="AA211" s="19"/>
+      <c r="AB211" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB211" s="2"/>
-    </row>
-    <row r="212" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC211" s="2"/>
+    </row>
+    <row r="212" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="5" t="s">
         <v>1522</v>
       </c>
@@ -23737,12 +23983,13 @@
       <c r="Z212" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA212" s="2" t="s">
+      <c r="AA212" s="19"/>
+      <c r="AB212" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB212" s="2"/>
-    </row>
-    <row r="213" spans="1:28" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC212" s="2"/>
+    </row>
+    <row r="213" spans="1:29" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="5" t="s">
         <v>1529</v>
       </c>
@@ -23801,12 +24048,13 @@
       <c r="Z213" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA213" s="2" t="s">
+      <c r="AA213" s="19"/>
+      <c r="AB213" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB213" s="2"/>
-    </row>
-    <row r="214" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC213" s="2"/>
+    </row>
+    <row r="214" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="5" t="s">
         <v>1536</v>
       </c>
@@ -23865,12 +24113,13 @@
       <c r="Z214" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA214" s="2" t="s">
+      <c r="AA214" s="19"/>
+      <c r="AB214" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB214" s="2"/>
-    </row>
-    <row r="215" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC214" s="2"/>
+    </row>
+    <row r="215" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="5" t="s">
         <v>1543</v>
       </c>
@@ -23929,12 +24178,13 @@
       <c r="Z215" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA215" s="2" t="s">
+      <c r="AA215" s="19"/>
+      <c r="AB215" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB215" s="2"/>
-    </row>
-    <row r="216" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC215" s="2"/>
+    </row>
+    <row r="216" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="5" t="s">
         <v>1550</v>
       </c>
@@ -23993,12 +24243,13 @@
       <c r="Z216" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA216" s="2" t="s">
+      <c r="AA216" s="19"/>
+      <c r="AB216" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB216" s="2"/>
-    </row>
-    <row r="217" spans="1:28" ht="288" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC216" s="2"/>
+    </row>
+    <row r="217" spans="1:29" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="5" t="s">
         <v>1557</v>
       </c>
@@ -24057,12 +24308,13 @@
       <c r="Z217" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA217" s="2" t="s">
+      <c r="AA217" s="19"/>
+      <c r="AB217" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB217" s="2"/>
-    </row>
-    <row r="218" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC217" s="2"/>
+    </row>
+    <row r="218" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="5" t="s">
         <v>1564</v>
       </c>
@@ -24121,12 +24373,13 @@
       <c r="Z218" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA218" s="2" t="s">
+      <c r="AA218" s="19"/>
+      <c r="AB218" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB218" s="2"/>
-    </row>
-    <row r="219" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC218" s="2"/>
+    </row>
+    <row r="219" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="5" t="s">
         <v>1571</v>
       </c>
@@ -24185,12 +24438,13 @@
       <c r="Z219" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA219" s="2" t="s">
+      <c r="AA219" s="19"/>
+      <c r="AB219" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB219" s="2"/>
-    </row>
-    <row r="220" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC219" s="2"/>
+    </row>
+    <row r="220" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="5" t="s">
         <v>1578</v>
       </c>
@@ -24249,12 +24503,13 @@
       <c r="Z220" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA220" s="2" t="s">
+      <c r="AA220" s="19"/>
+      <c r="AB220" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB220" s="2"/>
-    </row>
-    <row r="221" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC220" s="2"/>
+    </row>
+    <row r="221" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="5" t="s">
         <v>1585</v>
       </c>
@@ -24313,12 +24568,13 @@
       <c r="Z221" s="14" t="s">
         <v>1818</v>
       </c>
-      <c r="AA221" s="2" t="s">
+      <c r="AA221" s="19"/>
+      <c r="AB221" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB221" s="2"/>
-    </row>
-    <row r="222" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC221" s="2"/>
+    </row>
+    <row r="222" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="5" t="s">
         <v>1594</v>
       </c>
@@ -24377,12 +24633,13 @@
       <c r="Z222" s="14" t="s">
         <v>1818</v>
       </c>
-      <c r="AA222" s="2" t="s">
+      <c r="AA222" s="19"/>
+      <c r="AB222" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB222" s="2"/>
-    </row>
-    <row r="223" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC222" s="2"/>
+    </row>
+    <row r="223" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="5" t="s">
         <v>1600</v>
       </c>
@@ -24441,12 +24698,13 @@
       <c r="Z223" s="14" t="s">
         <v>1818</v>
       </c>
-      <c r="AA223" s="2" t="s">
+      <c r="AA223" s="19"/>
+      <c r="AB223" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB223" s="2"/>
-    </row>
-    <row r="224" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC223" s="2"/>
+    </row>
+    <row r="224" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="5" t="s">
         <v>1606</v>
       </c>
@@ -24505,12 +24763,13 @@
       <c r="Z224" s="14" t="s">
         <v>1818</v>
       </c>
-      <c r="AA224" s="2" t="s">
+      <c r="AA224" s="19"/>
+      <c r="AB224" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB224" s="2"/>
-    </row>
-    <row r="225" spans="1:28" ht="388.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC224" s="2"/>
+    </row>
+    <row r="225" spans="1:29" ht="388.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="7" t="s">
         <v>1612</v>
       </c>
@@ -24569,12 +24828,13 @@
       <c r="Z225" s="14" t="s">
         <v>1778</v>
       </c>
-      <c r="AA225" s="2" t="s">
+      <c r="AA225" s="19"/>
+      <c r="AB225" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB225" s="2"/>
-    </row>
-    <row r="226" spans="1:28" ht="403.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC225" s="2"/>
+    </row>
+    <row r="226" spans="1:29" ht="403.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="7" t="s">
         <v>1618</v>
       </c>
@@ -24633,12 +24893,13 @@
       <c r="Z226" s="14" t="s">
         <v>1778</v>
       </c>
-      <c r="AA226" s="2" t="s">
+      <c r="AA226" s="19"/>
+      <c r="AB226" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB226" s="2"/>
-    </row>
-    <row r="227" spans="1:28" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC226" s="2"/>
+    </row>
+    <row r="227" spans="1:29" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="5" t="s">
         <v>1624</v>
       </c>
@@ -24697,12 +24958,13 @@
       <c r="Z227" s="14" t="s">
         <v>1779</v>
       </c>
-      <c r="AA227" s="2" t="s">
+      <c r="AA227" s="19"/>
+      <c r="AB227" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB227" s="2"/>
-    </row>
-    <row r="228" spans="1:28" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC227" s="2"/>
+    </row>
+    <row r="228" spans="1:29" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="5" t="s">
         <v>1631</v>
       </c>
@@ -24761,12 +25023,13 @@
       <c r="Z228" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA228" s="2" t="s">
+      <c r="AA228" s="19"/>
+      <c r="AB228" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB228" s="2"/>
-    </row>
-    <row r="229" spans="1:28" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC228" s="2"/>
+    </row>
+    <row r="229" spans="1:29" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="7" t="s">
         <v>1638</v>
       </c>
@@ -24825,12 +25088,13 @@
       <c r="Z229" s="15" t="s">
         <v>1803</v>
       </c>
-      <c r="AA229" s="2" t="s">
+      <c r="AA229" s="20"/>
+      <c r="AB229" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB229" s="2"/>
-    </row>
-    <row r="230" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC229" s="2"/>
+    </row>
+    <row r="230" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="5" t="s">
         <v>1645</v>
       </c>
@@ -24889,12 +25153,13 @@
       <c r="Z230" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA230" s="2" t="s">
+      <c r="AA230" s="19"/>
+      <c r="AB230" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB230" s="2"/>
-    </row>
-    <row r="231" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC230" s="2"/>
+    </row>
+    <row r="231" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="5" t="s">
         <v>1652</v>
       </c>
@@ -24953,12 +25218,13 @@
       <c r="Z231" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA231" s="2" t="s">
+      <c r="AA231" s="19"/>
+      <c r="AB231" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB231" s="2"/>
-    </row>
-    <row r="232" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC231" s="2"/>
+    </row>
+    <row r="232" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="5" t="s">
         <v>1658</v>
       </c>
@@ -25017,12 +25283,13 @@
       <c r="Z232" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA232" s="2" t="s">
+      <c r="AA232" s="19"/>
+      <c r="AB232" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB232" s="2"/>
-    </row>
-    <row r="233" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC232" s="2"/>
+    </row>
+    <row r="233" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="5" t="s">
         <v>1664</v>
       </c>
@@ -25081,12 +25348,13 @@
       <c r="Z233" s="14" t="s">
         <v>1806</v>
       </c>
-      <c r="AA233" s="2" t="s">
+      <c r="AA233" s="19"/>
+      <c r="AB233" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB233" s="2"/>
-    </row>
-    <row r="234" spans="1:28" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC233" s="2"/>
+    </row>
+    <row r="234" spans="1:29" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="5" t="s">
         <v>1670</v>
       </c>
@@ -25145,12 +25413,13 @@
       <c r="Z234" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA234" s="2" t="s">
+      <c r="AA234" s="19"/>
+      <c r="AB234" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB234" s="2"/>
-    </row>
-    <row r="235" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC234" s="2"/>
+    </row>
+    <row r="235" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="7" t="s">
         <v>1676</v>
       </c>
@@ -25209,12 +25478,13 @@
       <c r="Z235" s="16" t="s">
         <v>1827</v>
       </c>
-      <c r="AA235" s="2" t="s">
+      <c r="AA235" s="21"/>
+      <c r="AB235" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB235" s="2"/>
-    </row>
-    <row r="236" spans="1:28" ht="403.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC235" s="2"/>
+    </row>
+    <row r="236" spans="1:29" ht="403.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="5" t="s">
         <v>1685</v>
       </c>
@@ -25273,12 +25543,13 @@
       <c r="Z236" s="14" t="s">
         <v>1818</v>
       </c>
-      <c r="AA236" s="2" t="s">
+      <c r="AA236" s="19"/>
+      <c r="AB236" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB236" s="2"/>
-    </row>
-    <row r="237" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC236" s="2"/>
+    </row>
+    <row r="237" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="7" t="s">
         <v>1692</v>
       </c>
@@ -25337,12 +25608,13 @@
       <c r="Z237" s="14" t="s">
         <v>1819</v>
       </c>
-      <c r="AA237" s="2" t="s">
+      <c r="AA237" s="19"/>
+      <c r="AB237" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB237" s="2"/>
-    </row>
-    <row r="238" spans="1:28" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC237" s="2"/>
+    </row>
+    <row r="238" spans="1:29" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="5" t="s">
         <v>1701</v>
       </c>
@@ -25401,12 +25673,13 @@
       <c r="Z238" s="14" t="s">
         <v>1785</v>
       </c>
-      <c r="AA238" s="2" t="s">
+      <c r="AA238" s="19"/>
+      <c r="AB238" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB238" s="2"/>
-    </row>
-    <row r="239" spans="1:28" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC238" s="2"/>
+    </row>
+    <row r="239" spans="1:29" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="5" t="s">
         <v>1708</v>
       </c>
@@ -25465,12 +25738,13 @@
       <c r="Z239" s="14" t="s">
         <v>1780</v>
       </c>
-      <c r="AA239" s="2" t="s">
+      <c r="AA239" s="19"/>
+      <c r="AB239" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AB239" s="2"/>
-    </row>
-    <row r="240" spans="1:28" ht="403.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC239" s="2"/>
+    </row>
+    <row r="240" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="13" t="s">
         <v>1835</v>
       </c>
@@ -25525,10 +25799,11 @@
       <c r="Z240" s="17" t="s">
         <v>1778</v>
       </c>
-      <c r="AA240" s="4"/>
+      <c r="AA240" s="22"/>
       <c r="AB240" s="4"/>
-    </row>
-    <row r="241" spans="1:28" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC240" s="4"/>
+    </row>
+    <row r="241" spans="1:29" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="13" t="s">
         <v>1842</v>
       </c>
@@ -25583,10 +25858,11 @@
       <c r="Z241" s="17" t="s">
         <v>1778</v>
       </c>
-      <c r="AA241" s="4"/>
+      <c r="AA241" s="22"/>
       <c r="AB241" s="4"/>
-    </row>
-    <row r="242" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC241" s="4"/>
+    </row>
+    <row r="242" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="13" t="s">
         <v>1848</v>
       </c>
@@ -25641,10 +25917,11 @@
       <c r="Z242" s="17" t="s">
         <v>1806</v>
       </c>
-      <c r="AA242" s="4"/>
+      <c r="AA242" s="22"/>
       <c r="AB242" s="4"/>
-    </row>
-    <row r="243" spans="1:28" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC242" s="4"/>
+    </row>
+    <row r="243" spans="1:29" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="13" t="s">
         <v>1854</v>
       </c>
@@ -25699,12 +25976,13 @@
       <c r="Z243" s="17" t="s">
         <v>1806</v>
       </c>
-      <c r="AA243" s="4"/>
+      <c r="AA243" s="22"/>
       <c r="AB243" s="4"/>
+      <c r="AC243" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB243" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD239">
+  <autoFilter ref="A1:AC243" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE239">
     <sortCondition ref="A2:A239"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>